<commit_message>
updated divisions and predictions
</commit_message>
<xml_diff>
--- a/finalscore_newleagues.xlsx
+++ b/finalscore_newleagues.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19018" uniqueCount="5133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18835" uniqueCount="5133">
   <si>
     <t>HT</t>
   </si>
@@ -90202,17 +90202,17 @@
       <c r="F2336" t="n" s="2">
         <v>44544.0</v>
       </c>
-      <c r="G2336" t="s">
-        <v>2583</v>
-      </c>
-      <c r="H2336" t="s">
-        <v>2471</v>
-      </c>
-      <c r="I2336" t="s">
-        <v>5090</v>
-      </c>
-      <c r="J2336" t="n">
-        <v>4.0</v>
+      <c r="G2336" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2336" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2336" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2336" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2337">
@@ -90234,17 +90234,17 @@
       <c r="F2337" t="n" s="2">
         <v>44544.0</v>
       </c>
-      <c r="G2337" t="s">
-        <v>2438</v>
-      </c>
-      <c r="H2337" t="s">
-        <v>2437</v>
-      </c>
-      <c r="I2337" t="s">
-        <v>5092</v>
-      </c>
-      <c r="J2337" t="n">
-        <v>0.0</v>
+      <c r="G2337" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2337" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2337" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2337" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2338">
@@ -90266,17 +90266,17 @@
       <c r="F2338" t="n" s="2">
         <v>44544.0</v>
       </c>
-      <c r="G2338" t="s">
-        <v>2531</v>
-      </c>
-      <c r="H2338" t="s">
-        <v>2532</v>
-      </c>
-      <c r="I2338" t="s">
-        <v>5092</v>
-      </c>
-      <c r="J2338" t="n">
-        <v>0.0</v>
+      <c r="G2338" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2338" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2338" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2338" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2339">
@@ -90298,17 +90298,17 @@
       <c r="F2339" t="n" s="2">
         <v>44544.0</v>
       </c>
-      <c r="G2339" t="s">
-        <v>2608</v>
-      </c>
-      <c r="H2339" t="s">
-        <v>2672</v>
-      </c>
-      <c r="I2339" t="s">
-        <v>5089</v>
-      </c>
-      <c r="J2339" t="n">
-        <v>4.0</v>
+      <c r="G2339" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2339" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2339" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2339" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2340">
@@ -90330,17 +90330,17 @@
       <c r="F2340" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2340" t="s">
-        <v>2592</v>
-      </c>
-      <c r="H2340" t="s">
-        <v>2574</v>
-      </c>
-      <c r="I2340" t="s">
-        <v>5093</v>
-      </c>
-      <c r="J2340" t="n">
-        <v>1.0</v>
+      <c r="G2340" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2340" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2340" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2340" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2341">
@@ -90362,17 +90362,17 @@
       <c r="F2341" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2341" t="s">
-        <v>2641</v>
-      </c>
-      <c r="H2341" t="s">
-        <v>2674</v>
-      </c>
-      <c r="I2341" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2341" t="n">
-        <v>2.0</v>
+      <c r="G2341" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2341" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2341" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2341" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2342">
@@ -90394,17 +90394,17 @@
       <c r="F2342" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2342" t="s">
-        <v>2424</v>
-      </c>
-      <c r="H2342" t="s">
-        <v>2595</v>
-      </c>
-      <c r="I2342" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2342" t="n">
-        <v>2.0</v>
+      <c r="G2342" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2342" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2342" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2342" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2343">
@@ -90426,17 +90426,17 @@
       <c r="F2343" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2343" t="s">
-        <v>2673</v>
-      </c>
-      <c r="H2343" t="s">
-        <v>2460</v>
-      </c>
-      <c r="I2343" t="s">
-        <v>5128</v>
-      </c>
-      <c r="J2343" t="n">
-        <v>7.0</v>
+      <c r="G2343" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2343" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2343" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2343" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2344">
@@ -90490,17 +90490,17 @@
       <c r="F2345" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2345" t="s">
-        <v>2666</v>
-      </c>
-      <c r="H2345" t="s">
-        <v>2565</v>
-      </c>
-      <c r="I2345" t="s">
-        <v>5102</v>
-      </c>
-      <c r="J2345" t="n">
-        <v>3.0</v>
+      <c r="G2345" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2345" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2345" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2345" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2346">
@@ -90522,17 +90522,17 @@
       <c r="F2346" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2346" t="s">
-        <v>2436</v>
-      </c>
-      <c r="H2346" t="s">
-        <v>2564</v>
-      </c>
-      <c r="I2346" t="s">
-        <v>5101</v>
-      </c>
-      <c r="J2346" t="n">
-        <v>4.0</v>
+      <c r="G2346" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2346" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2346" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2346" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2347">
@@ -90554,17 +90554,17 @@
       <c r="F2347" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2347" t="s">
-        <v>2599</v>
-      </c>
-      <c r="H2347" t="s">
-        <v>2566</v>
-      </c>
-      <c r="I2347" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2347" t="n">
-        <v>3.0</v>
+      <c r="G2347" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2347" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2347" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2347" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2348">
@@ -90586,17 +90586,17 @@
       <c r="F2348" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2348" t="s">
-        <v>2410</v>
-      </c>
-      <c r="H2348" t="s">
-        <v>2551</v>
-      </c>
-      <c r="I2348" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2348" t="n">
-        <v>2.0</v>
+      <c r="G2348" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2348" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2348" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2348" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2349">
@@ -90618,17 +90618,17 @@
       <c r="F2349" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2349" t="s">
-        <v>2475</v>
-      </c>
-      <c r="H2349" t="s">
-        <v>2567</v>
-      </c>
-      <c r="I2349" t="s">
-        <v>5096</v>
-      </c>
-      <c r="J2349" t="n">
-        <v>4.0</v>
+      <c r="G2349" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2349" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2349" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2349" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2350">
@@ -90650,17 +90650,17 @@
       <c r="F2350" t="n" s="2">
         <v>44545.0</v>
       </c>
-      <c r="G2350" t="s">
-        <v>2588</v>
-      </c>
-      <c r="H2350" t="s">
-        <v>2536</v>
-      </c>
-      <c r="I2350" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2350" t="n">
-        <v>2.0</v>
+      <c r="G2350" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2350" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2350" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2350" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2351">
@@ -90682,17 +90682,17 @@
       <c r="F2351" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2351" t="s">
-        <v>2593</v>
-      </c>
-      <c r="H2351" t="s">
-        <v>2575</v>
-      </c>
-      <c r="I2351" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2351" t="n">
-        <v>2.0</v>
+      <c r="G2351" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2351" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2351" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2351" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2352">
@@ -90714,17 +90714,17 @@
       <c r="F2352" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2352" t="s">
-        <v>2422</v>
-      </c>
-      <c r="H2352" t="s">
-        <v>2462</v>
-      </c>
-      <c r="I2352" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2352" t="n">
-        <v>3.0</v>
+      <c r="G2352" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2352" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2352" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2352" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2353">
@@ -90746,17 +90746,17 @@
       <c r="F2353" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2353" t="s">
-        <v>2459</v>
-      </c>
-      <c r="H2353" t="s">
-        <v>2423</v>
-      </c>
-      <c r="I2353" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2353" t="n">
-        <v>2.0</v>
+      <c r="G2353" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2353" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2353" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2353" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2354">
@@ -90778,17 +90778,17 @@
       <c r="F2354" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2354" t="s">
-        <v>2461</v>
-      </c>
-      <c r="H2354" t="s">
-        <v>2425</v>
-      </c>
-      <c r="I2354" t="s">
-        <v>5088</v>
-      </c>
-      <c r="J2354" t="n">
-        <v>1.0</v>
+      <c r="G2354" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2354" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2354" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2354" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2355">
@@ -90810,17 +90810,17 @@
       <c r="F2355" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2355" t="s">
-        <v>2502</v>
-      </c>
-      <c r="H2355" t="s">
-        <v>2503</v>
-      </c>
-      <c r="I2355" t="s">
-        <v>5100</v>
-      </c>
-      <c r="J2355" t="n">
-        <v>3.0</v>
+      <c r="G2355" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2355" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2355" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2355" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2356">
@@ -90842,17 +90842,17 @@
       <c r="F2356" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2356" t="s">
-        <v>2411</v>
-      </c>
-      <c r="H2356" t="s">
-        <v>2552</v>
-      </c>
-      <c r="I2356" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2356" t="n">
-        <v>3.0</v>
+      <c r="G2356" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2356" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2356" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2356" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2357">
@@ -90874,17 +90874,17 @@
       <c r="F2357" t="n" s="2">
         <v>44546.0</v>
       </c>
-      <c r="G2357" t="s">
-        <v>2474</v>
-      </c>
-      <c r="H2357" t="s">
-        <v>2584</v>
-      </c>
-      <c r="I2357" t="s">
-        <v>5094</v>
-      </c>
-      <c r="J2357" t="n">
-        <v>2.0</v>
+      <c r="G2357" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2357" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2357" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2357" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2358">
@@ -90906,17 +90906,17 @@
       <c r="F2358" t="n" s="2">
         <v>44547.0</v>
       </c>
-      <c r="G2358" t="s">
-        <v>2501</v>
-      </c>
-      <c r="H2358" t="s">
-        <v>2408</v>
-      </c>
-      <c r="I2358" t="s">
-        <v>5105</v>
-      </c>
-      <c r="J2358" t="n">
-        <v>3.0</v>
+      <c r="G2358" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2358" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2358" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2358" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2359">
@@ -90938,17 +90938,17 @@
       <c r="F2359" t="n" s="2">
         <v>44547.0</v>
       </c>
-      <c r="G2359" t="s">
-        <v>2637</v>
-      </c>
-      <c r="H2359" t="s">
-        <v>2550</v>
-      </c>
-      <c r="I2359" t="s">
-        <v>5088</v>
-      </c>
-      <c r="J2359" t="n">
-        <v>1.0</v>
+      <c r="G2359" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2359" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2359" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2359" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2360">
@@ -90970,17 +90970,17 @@
       <c r="F2360" t="n" s="2">
         <v>44547.0</v>
       </c>
-      <c r="G2360" t="s">
-        <v>2437</v>
-      </c>
-      <c r="H2360" t="s">
-        <v>2532</v>
-      </c>
-      <c r="I2360" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2360" t="n">
-        <v>3.0</v>
+      <c r="G2360" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2360" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2360" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2360" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2361">
@@ -91002,17 +91002,17 @@
       <c r="F2361" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2361" t="s">
-        <v>2574</v>
-      </c>
-      <c r="H2361" t="s">
-        <v>2424</v>
-      </c>
-      <c r="I2361" t="s">
-        <v>5102</v>
-      </c>
-      <c r="J2361" t="n">
-        <v>3.0</v>
+      <c r="G2361" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2361" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2361" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2361" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2362">
@@ -91034,17 +91034,17 @@
       <c r="F2362" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2362" t="s">
-        <v>2674</v>
-      </c>
-      <c r="H2362" t="s">
-        <v>2673</v>
-      </c>
-      <c r="I2362" t="s">
-        <v>5102</v>
-      </c>
-      <c r="J2362" t="n">
-        <v>3.0</v>
+      <c r="G2362" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2362" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2362" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2362" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2363">
@@ -91066,17 +91066,17 @@
       <c r="F2363" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2363" t="s">
-        <v>2595</v>
-      </c>
-      <c r="H2363" t="s">
-        <v>2592</v>
-      </c>
-      <c r="I2363" t="s">
-        <v>5108</v>
-      </c>
-      <c r="J2363" t="n">
-        <v>5.0</v>
+      <c r="G2363" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2363" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2363" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2363" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2364">
@@ -91098,17 +91098,17 @@
       <c r="F2364" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2364" t="s">
-        <v>2460</v>
-      </c>
-      <c r="H2364" t="s">
-        <v>2641</v>
-      </c>
-      <c r="I2364" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2364" t="n">
-        <v>2.0</v>
+      <c r="G2364" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2364" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2364" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2364" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2365">
@@ -91130,17 +91130,17 @@
       <c r="F2365" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2365" t="s">
-        <v>2471</v>
-      </c>
-      <c r="H2365" t="s">
-        <v>2582</v>
-      </c>
-      <c r="I2365" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2365" t="n">
-        <v>2.0</v>
+      <c r="G2365" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2365" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2365" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2365" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2366">
@@ -91162,17 +91162,17 @@
       <c r="F2366" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2366" t="s">
-        <v>2473</v>
-      </c>
-      <c r="H2366" t="s">
-        <v>2529</v>
-      </c>
-      <c r="I2366" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2366" t="n">
-        <v>2.0</v>
+      <c r="G2366" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2366" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2366" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2366" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2367">
@@ -91194,17 +91194,17 @@
       <c r="F2367" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2367" t="s">
-        <v>2472</v>
-      </c>
-      <c r="H2367" t="s">
-        <v>2530</v>
-      </c>
-      <c r="I2367" t="s">
-        <v>5094</v>
-      </c>
-      <c r="J2367" t="n">
-        <v>2.0</v>
+      <c r="G2367" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2367" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2367" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2367" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2368">
@@ -91226,17 +91226,17 @@
       <c r="F2368" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2368" t="s">
-        <v>2666</v>
-      </c>
-      <c r="H2368" t="s">
-        <v>2435</v>
-      </c>
-      <c r="I2368" t="s">
-        <v>5109</v>
-      </c>
-      <c r="J2368" t="n">
-        <v>5.0</v>
+      <c r="G2368" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2368" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2368" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2368" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2369">
@@ -91258,17 +91258,17 @@
       <c r="F2369" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2369" t="s">
-        <v>2566</v>
-      </c>
-      <c r="H2369" t="s">
-        <v>2531</v>
-      </c>
-      <c r="I2369" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2369" t="n">
-        <v>2.0</v>
+      <c r="G2369" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2369" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2369" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2369" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2370">
@@ -91290,17 +91290,17 @@
       <c r="F2370" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2370" t="s">
-        <v>2567</v>
-      </c>
-      <c r="H2370" t="s">
-        <v>2599</v>
-      </c>
-      <c r="I2370" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2370" t="n">
-        <v>2.0</v>
+      <c r="G2370" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2370" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2370" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2370" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2371">
@@ -91322,17 +91322,17 @@
       <c r="F2371" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2371" t="s">
-        <v>2587</v>
-      </c>
-      <c r="H2371" t="s">
-        <v>2535</v>
-      </c>
-      <c r="I2371" t="s">
-        <v>5096</v>
-      </c>
-      <c r="J2371" t="n">
-        <v>4.0</v>
+      <c r="G2371" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2371" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2371" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2371" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2372">
@@ -91354,17 +91354,17 @@
       <c r="F2372" t="n" s="2">
         <v>44548.0</v>
       </c>
-      <c r="G2372" t="s">
-        <v>2444</v>
-      </c>
-      <c r="H2372" t="s">
-        <v>2537</v>
-      </c>
-      <c r="I2372" t="s">
-        <v>5094</v>
-      </c>
-      <c r="J2372" t="n">
-        <v>2.0</v>
+      <c r="G2372" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2372" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2372" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2372" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2373">
@@ -91386,17 +91386,17 @@
       <c r="F2373" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2373" t="s">
-        <v>2434</v>
-      </c>
-      <c r="H2373" t="s">
-        <v>2564</v>
-      </c>
-      <c r="I2373" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2373" t="n">
-        <v>3.0</v>
+      <c r="G2373" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2373" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2373" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2373" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2374">
@@ -91418,17 +91418,17 @@
       <c r="F2374" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2374" t="s">
-        <v>2409</v>
-      </c>
-      <c r="H2374" t="s">
-        <v>2565</v>
-      </c>
-      <c r="I2374" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2374" t="n">
-        <v>3.0</v>
+      <c r="G2374" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2374" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2374" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2374" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2375">
@@ -91450,17 +91450,17 @@
       <c r="F2375" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2375" t="s">
-        <v>2436</v>
-      </c>
-      <c r="H2375" t="s">
-        <v>2583</v>
-      </c>
-      <c r="I2375" t="s">
-        <v>5100</v>
-      </c>
-      <c r="J2375" t="n">
-        <v>3.0</v>
+      <c r="G2375" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2375" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2375" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2375" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2376">
@@ -91482,17 +91482,17 @@
       <c r="F2376" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2376" t="s">
-        <v>2438</v>
-      </c>
-      <c r="H2376" t="s">
-        <v>2502</v>
-      </c>
-      <c r="I2376" t="s">
-        <v>5093</v>
-      </c>
-      <c r="J2376" t="n">
-        <v>1.0</v>
+      <c r="G2376" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2376" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2376" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2376" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2377">
@@ -91514,17 +91514,17 @@
       <c r="F2377" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2377" t="s">
-        <v>2584</v>
-      </c>
-      <c r="H2377" t="s">
-        <v>2410</v>
-      </c>
-      <c r="I2377" t="s">
-        <v>5088</v>
-      </c>
-      <c r="J2377" t="n">
-        <v>1.0</v>
+      <c r="G2377" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2377" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2377" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2377" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2378">
@@ -91546,17 +91546,17 @@
       <c r="F2378" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2378" t="s">
-        <v>2551</v>
-      </c>
-      <c r="H2378" t="s">
-        <v>2475</v>
-      </c>
-      <c r="I2378" t="s">
-        <v>5092</v>
-      </c>
-      <c r="J2378" t="n">
-        <v>0.0</v>
+      <c r="G2378" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2378" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2378" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2378" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2379">
@@ -91578,17 +91578,17 @@
       <c r="F2379" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2379" t="s">
-        <v>2482</v>
-      </c>
-      <c r="H2379" t="s">
-        <v>2588</v>
-      </c>
-      <c r="I2379" t="s">
-        <v>5114</v>
-      </c>
-      <c r="J2379" t="n">
-        <v>5.0</v>
+      <c r="G2379" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2379" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2379" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2379" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2380">
@@ -91610,17 +91610,17 @@
       <c r="F2380" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2380" t="s">
-        <v>2536</v>
-      </c>
-      <c r="H2380" t="s">
-        <v>2483</v>
-      </c>
-      <c r="I2380" t="s">
-        <v>5090</v>
-      </c>
-      <c r="J2380" t="n">
-        <v>4.0</v>
+      <c r="G2380" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2380" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2380" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2380" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2381">
@@ -91642,17 +91642,17 @@
       <c r="F2381" t="n" s="2">
         <v>44549.0</v>
       </c>
-      <c r="G2381" t="s">
-        <v>2484</v>
-      </c>
-      <c r="H2381" t="s">
-        <v>2445</v>
-      </c>
-      <c r="I2381" t="s">
-        <v>5097</v>
-      </c>
-      <c r="J2381" t="n">
-        <v>2.0</v>
+      <c r="G2381" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2381" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2381" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2381" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2382">
@@ -91674,17 +91674,17 @@
       <c r="F2382" t="n" s="2">
         <v>44550.0</v>
       </c>
-      <c r="G2382" t="s">
-        <v>2503</v>
-      </c>
-      <c r="H2382" t="s">
-        <v>2411</v>
-      </c>
-      <c r="I2382" t="s">
-        <v>5092</v>
-      </c>
-      <c r="J2382" t="n">
-        <v>0.0</v>
+      <c r="G2382" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2382" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2382" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2382" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2383">
@@ -91706,17 +91706,17 @@
       <c r="F2383" t="n" s="2">
         <v>44550.0</v>
       </c>
-      <c r="G2383" t="s">
-        <v>2552</v>
-      </c>
-      <c r="H2383" t="s">
-        <v>2474</v>
-      </c>
-      <c r="I2383" t="s">
-        <v>5094</v>
-      </c>
-      <c r="J2383" t="n">
-        <v>2.0</v>
+      <c r="G2383" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2383" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2383" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2383" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2384">
@@ -91738,17 +91738,17 @@
       <c r="F2384" t="n" s="2">
         <v>44551.0</v>
       </c>
-      <c r="G2384" t="s">
-        <v>2424</v>
-      </c>
-      <c r="H2384" t="s">
-        <v>2674</v>
-      </c>
-      <c r="I2384" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2384" t="n">
-        <v>3.0</v>
+      <c r="G2384" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2384" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2384" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2384" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2385">
@@ -91770,17 +91770,17 @@
       <c r="F2385" t="n" s="2">
         <v>44551.0</v>
       </c>
-      <c r="G2385" t="s">
-        <v>2673</v>
-      </c>
-      <c r="H2385" t="s">
-        <v>2574</v>
-      </c>
-      <c r="I2385" t="s">
-        <v>5102</v>
-      </c>
-      <c r="J2385" t="n">
-        <v>3.0</v>
+      <c r="G2385" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2385" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2385" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2385" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2386">
@@ -91802,17 +91802,17 @@
       <c r="F2386" t="n" s="2">
         <v>44552.0</v>
       </c>
-      <c r="G2386" t="s">
-        <v>2462</v>
-      </c>
-      <c r="H2386" t="s">
-        <v>2423</v>
-      </c>
-      <c r="I2386" t="s">
-        <v>5090</v>
-      </c>
-      <c r="J2386" t="n">
-        <v>4.0</v>
+      <c r="G2386" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2386" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2386" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2386" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2387">
@@ -91834,17 +91834,17 @@
       <c r="F2387" t="n" s="2">
         <v>44552.0</v>
       </c>
-      <c r="G2387" t="s">
-        <v>2575</v>
-      </c>
-      <c r="H2387" t="s">
-        <v>2425</v>
-      </c>
-      <c r="I2387" t="s">
-        <v>5091</v>
-      </c>
-      <c r="J2387" t="n">
-        <v>2.0</v>
+      <c r="G2387" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2387" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2387" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2387" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2388">
@@ -91866,17 +91866,17 @@
       <c r="F2388" t="n" s="2">
         <v>44552.0</v>
       </c>
-      <c r="G2388" t="s">
-        <v>2593</v>
-      </c>
-      <c r="H2388" t="s">
-        <v>2461</v>
-      </c>
-      <c r="I2388" t="s">
-        <v>5092</v>
-      </c>
-      <c r="J2388" t="n">
-        <v>0.0</v>
+      <c r="G2388" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2388" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2388" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2388" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2389">
@@ -91898,17 +91898,17 @@
       <c r="F2389" t="n" s="2">
         <v>44552.0</v>
       </c>
-      <c r="G2389" t="s">
-        <v>2422</v>
-      </c>
-      <c r="H2389" t="s">
-        <v>2459</v>
-      </c>
-      <c r="I2389" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2389" t="n">
-        <v>3.0</v>
+      <c r="G2389" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2389" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2389" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2389" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2390">
@@ -91930,17 +91930,17 @@
       <c r="F2390" t="n" s="2">
         <v>44555.0</v>
       </c>
-      <c r="G2390" t="s">
-        <v>2424</v>
-      </c>
-      <c r="H2390" t="s">
-        <v>2460</v>
-      </c>
-      <c r="I2390" t="s">
-        <v>5097</v>
-      </c>
-      <c r="J2390" t="n">
-        <v>2.0</v>
+      <c r="G2390" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2390" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2390" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2390" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2391">
@@ -91962,17 +91962,17 @@
       <c r="F2391" t="n" s="2">
         <v>44555.0</v>
       </c>
-      <c r="G2391" t="s">
-        <v>2673</v>
-      </c>
-      <c r="H2391" t="s">
-        <v>2595</v>
-      </c>
-      <c r="I2391" t="s">
-        <v>5093</v>
-      </c>
-      <c r="J2391" t="n">
-        <v>1.0</v>
+      <c r="G2391" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2391" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2391" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2391" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2392">
@@ -91994,17 +91994,17 @@
       <c r="F2392" t="n" s="2">
         <v>44555.0</v>
       </c>
-      <c r="G2392" t="s">
-        <v>2592</v>
-      </c>
-      <c r="H2392" t="s">
-        <v>2674</v>
-      </c>
-      <c r="I2392" t="s">
-        <v>5093</v>
-      </c>
-      <c r="J2392" t="n">
-        <v>1.0</v>
+      <c r="G2392" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2392" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2392" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2392" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2393">
@@ -92026,17 +92026,17 @@
       <c r="F2393" t="n" s="2">
         <v>44555.0</v>
       </c>
-      <c r="G2393" t="s">
-        <v>2641</v>
-      </c>
-      <c r="H2393" t="s">
-        <v>2574</v>
-      </c>
-      <c r="I2393" t="s">
-        <v>5088</v>
-      </c>
-      <c r="J2393" t="n">
-        <v>1.0</v>
+      <c r="G2393" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2393" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2393" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2393" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2394">
@@ -92058,17 +92058,17 @@
       <c r="F2394" t="n" s="2">
         <v>44556.0</v>
       </c>
-      <c r="G2394" t="s">
-        <v>2459</v>
-      </c>
-      <c r="H2394" t="s">
-        <v>2425</v>
-      </c>
-      <c r="I2394" t="s">
-        <v>5104</v>
-      </c>
-      <c r="J2394" t="n">
-        <v>3.0</v>
+      <c r="G2394" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2394" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2394" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2394" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2395">
@@ -92090,17 +92090,17 @@
       <c r="F2395" t="n" s="2">
         <v>44556.0</v>
       </c>
-      <c r="G2395" t="s">
-        <v>2461</v>
-      </c>
-      <c r="H2395" t="s">
-        <v>2423</v>
-      </c>
-      <c r="I2395" t="s">
-        <v>5096</v>
-      </c>
-      <c r="J2395" t="n">
-        <v>4.0</v>
+      <c r="G2395" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2395" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2395" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2395" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2396">
@@ -92122,17 +92122,17 @@
       <c r="F2396" t="n" s="2">
         <v>44556.0</v>
       </c>
-      <c r="G2396" t="s">
-        <v>2593</v>
-      </c>
-      <c r="H2396" t="s">
-        <v>2462</v>
-      </c>
-      <c r="I2396" t="s">
-        <v>5088</v>
-      </c>
-      <c r="J2396" t="n">
-        <v>1.0</v>
+      <c r="G2396" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2396" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2396" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2396" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="2397">
@@ -92154,17 +92154,17 @@
       <c r="F2397" t="n" s="2">
         <v>44556.0</v>
       </c>
-      <c r="G2397" t="s">
-        <v>2422</v>
-      </c>
-      <c r="H2397" t="s">
-        <v>2575</v>
-      </c>
-      <c r="I2397" t="s">
-        <v>5097</v>
-      </c>
-      <c r="J2397" t="n">
-        <v>2.0</v>
+      <c r="G2397" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H2397" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I2397" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J2397" t="e">
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>